<commit_message>
streamlit view, functions to type shop list
</commit_message>
<xml_diff>
--- a/server/lista.xlsx
+++ b/server/lista.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -917,156 +917,148 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Arroz Agulha</t>
+          <t>Ovos de Galinhas Criadas ao Ar Livre Classe M/L Pingo Doce 6 un</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>€1,69
-/un</t>
+          <t>1,59€ / un</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Continente</t>
+          <t>Pingo Doce</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Arroz Agulha</t>
+          <t>Ovos de Codorniz Pingo Doce 12 un</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>€1,59
-/un</t>
+          <t>1,30€ / un</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Continente</t>
+          <t>Pingo Doce</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Arroz Agulha</t>
+          <t>Ovos de Galinhas Criadas no Solo Classe L Pingo Doce 6 un</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>€1,33
-/un</t>
+          <t>1,48€ / un</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Continente</t>
+          <t>Pingo Doce</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Arroz Agulha</t>
+          <t>Ovos de Galinhas Criadas no Solo Classe L Pingo Doce 12 un</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>€1,38
-/un</t>
+          <t>2,48€ / un</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Continente</t>
+          <t>Pingo Doce</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Arroz Agulha Selecionado</t>
+          <t>Ovos de Galinhas Criadas no Solo Classe M Pingo Doce 6 un</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>€1,26
-/un</t>
+          <t>1,38€ / un</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Continente</t>
+          <t>Pingo Doce</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Arroz Agulha Europa</t>
+          <t>Ovos de Galinhas Criadas no Solo Classe M Pingo Doce 12 un</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>€1,18
-/un</t>
+          <t>2,33€ / un</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Continente</t>
+          <t>Pingo Doce</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Arroz Agulha Extra Longo</t>
+          <t>Ovos de Galinhas Criadas no Solo Classe XL Pingo Doce 6 un</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>€2,37
-/un</t>
+          <t>2,07€ / un</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Continente</t>
+          <t>Pingo Doce</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Arroz Agulha Extra Longo</t>
+          <t>Ovos Classe M/L Pingo Doce Biológico 6 un</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>€1,62
-/un</t>
+          <t>2,39€ / un</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Continente</t>
+          <t>Pingo Doce</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Arroz Agulha Europa Pack Poupança</t>
+          <t>Arroz Agulha</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>€1,36
+          <t>€1,69
 /un</t>
         </is>
       </c>
@@ -1079,12 +1071,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Arroz Agulha Branqueado Extra Longo</t>
+          <t>Arroz Agulha</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>€1,33
+          <t>€1,59
 /un</t>
         </is>
       </c>
@@ -1097,12 +1089,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Arroz Agulha Pronto a Comer</t>
+          <t>Arroz Agulha</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>€1,34
+          <t>€1,33
 /un</t>
         </is>
       </c>
@@ -1115,12 +1107,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Arroz Agulha Pronto a Comer sem Glúten</t>
+          <t>Arroz Agulha</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>€1,45
+          <t>€1,38
 /un</t>
         </is>
       </c>
@@ -1133,16 +1125,610 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
+          <t>Arroz Agulha Europa</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>€1,18
+/un</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Arroz Agulha Selecionado</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>€1,26
+/un</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Arroz Agulha Integral</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>€1,28
+/un</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Arroz Agulha Extra Longo</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>€2,37
+/un</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Arroz Agulha Extra Longo</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>€1,28
+/un</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Arroz Agulha Europa Pack Poupança</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>€1,36
+/un</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Arroz Agulha Branqueado Extra Longo</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>€1,33
+/un</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Arroz Agulha Pronto a Comer</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>€1,45
+/un</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Arroz Agulha Pronto a Comer sem Glúten</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>€1,45
+/un</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
           <t>Arroz Longo Comum</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B51" t="inlineStr">
         <is>
           <t>€1,08
 /un</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Ovos de Solo Classe L</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>€2,48
+/un</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Ovos de Solo Classe M</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>€2,33
+/un</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Ovos de Ar Livre Classe M/L</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>€3,74
+/un</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Ovos Classe M</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>€4,68
+/un</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Ovos de Ar Livre Classe M/L</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>€2,59
+/un</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Ovos de Ar Livre</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>€2,38
+/un</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Ovos de Solo Classe XL</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>€2,06
+/un</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Ovos de Codorniz</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>€1,30
+/un</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Ovos de Solo Classe M</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>€1,37
+/un</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Ovos de Solo Classe L</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>€1,48
+/un</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Ovos Classe M/L</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>€3,04
+/un</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Clara de Ovo Pasteurizada</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>€2,95
+/un</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Ovos de Ar Livre Classe M/L</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>€1,84
+/un</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Ovos de Ar Livre Classe M/L</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>€1,59
+/un</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Ovos de Solo Classe M/L</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>€3,94
+/un</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Ovos Classe L</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>€3,14
+/un</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Clara de Ovo Líquida Pasteurizada</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>€1,15
+/un</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Ovos Classe M</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>€3,04
+/un</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Ovos Classe M/L Ruby</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>€2,65
+/un</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Ovos de Solo Classe S</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>€1,18
+/un</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Ovos de Ar Livre Classe XL</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>€2,58
+/un</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Ovos de Solo Classe M</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>€3,15
+/un</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Clara de Ovo Proteína Baunilha</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>€1,84
+/un</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Clara de Ovo Proteína Morango</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>€1,84
+/un</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
         <is>
           <t>Continente</t>
         </is>

</xml_diff>